<commit_message>
Typography ders bölüm 1 bitti
</commit_message>
<xml_diff>
--- a/kelime.xlsx
+++ b/kelime.xlsx
@@ -19,15 +19,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>At first glance</t>
-  </si>
-  <si>
-    <t>ilk bakışta</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>spacious</t>
+  </si>
+  <si>
+    <t>geniş, ferah</t>
+  </si>
+  <si>
+    <t>sıfat</t>
+  </si>
+  <si>
+    <t>legibility</t>
   </si>
   <si>
     <t>isim</t>
+  </si>
+  <si>
+    <t>okunabilirlik</t>
   </si>
 </sst>
 </file>
@@ -353,26 +362,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:E6"/>
+  <dimension ref="C6:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:5" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>0</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
yeni kelime eklendi 28 ekim
</commit_message>
<xml_diff>
--- a/kelime.xlsx
+++ b/kelime.xlsx
@@ -21,13 +21,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>sıfat</t>
+    <t>intensity</t>
   </si>
   <si>
-    <t>interior</t>
+    <t>yoğunluk</t>
   </si>
   <si>
-    <t>iç, dahili</t>
+    <t>isim</t>
   </si>
 </sst>
 </file>
@@ -353,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:E11"/>
+  <dimension ref="C6:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,15 +368,15 @@
     <row r="6" spans="3:5" ht="20.25" x14ac:dyDescent="0.35">
       <c r="C6" s="1"/>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E12" t="s">
         <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>